<commit_message>
few changes in Automation flow
</commit_message>
<xml_diff>
--- a/customLibrary/getdata.xlsx
+++ b/customLibrary/getdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SatishKumar\PycharmProjects\POC_Doxa_RobotFrameWork\customLibrary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37440B6F-139E-47B6-AB25-CBB8CBB442F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B358A1B-D475-4B76-A18F-2B659E10A60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3C518E7A-1461-4509-9B57-60B89352E197}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="158">
   <si>
     <t>Username</t>
   </si>
@@ -377,9 +377,6 @@
     <t xml:space="preserve">Currency </t>
   </si>
   <si>
-    <t>(//div[@class="ag-center-cols-clipper"])[1]/div/div/div/div[@col-id="sourceCurrency"]</t>
-  </si>
-  <si>
     <t>Currency Option</t>
   </si>
   <si>
@@ -465,13 +462,61 @@
   </si>
   <si>
     <t>first list</t>
+  </si>
+  <si>
+    <t>Requisition left Tab</t>
+  </si>
+  <si>
+    <t>Raise Requisition</t>
+  </si>
+  <si>
+    <t>xpath://span[normalize-space()='Raise Requisition']</t>
+  </si>
+  <si>
+    <t>Raise Requisition Type of Requisition</t>
+  </si>
+  <si>
+    <t>Purchase Requisition</t>
+  </si>
+  <si>
+    <t>xpath://textarea[@placeholder='Enter PR Title']</t>
+  </si>
+  <si>
+    <t>PR_Title</t>
+  </si>
+  <si>
+    <t>Raise PR UOM code field</t>
+  </si>
+  <si>
+    <t>xpath:(//div[@col-id="uom"])[2]</t>
+  </si>
+  <si>
+    <t>xpath:(//div[@col-id="itemQuantity"])[2]</t>
+  </si>
+  <si>
+    <t>Raise PR item quantity</t>
+  </si>
+  <si>
+    <t>xpath:(//div[@class="ag-center-cols-clipper"])[1]/div/div/div/div[@col-id="sourceCurrency"]</t>
+  </si>
+  <si>
+    <t>xpath:(//div[@col-id="itemUnitPrice"])[2]</t>
+  </si>
+  <si>
+    <t>Item Unit Price</t>
+  </si>
+  <si>
+    <t>xpath:(//div[@col-id="priceType"])[2]</t>
+  </si>
+  <si>
+    <t>Price Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,6 +590,12 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -566,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -588,6 +639,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00092C5-C846-4B0A-8001-D507774B3722}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -920,9 +972,10 @@
     <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="45.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="43.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18">
+    <row r="1" spans="1:11" ht="18">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -951,10 +1004,13 @@
         <v>107</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>140</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -983,10 +1039,13 @@
         <v>109</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>139</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1002,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C177288E-979B-4494-9C30-0F44EC20F1D2}">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1320,7 +1379,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>90</v>
@@ -1411,111 +1470,167 @@
         <v>112</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>113</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
+        <v>113</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
+        <v>119</v>
+      </c>
+      <c r="B54" t="s">
         <v>120</v>
-      </c>
-      <c r="B54" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
+        <v>121</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
+        <v>135</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
+        <v>137</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>139</v>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>142</v>
+      </c>
+      <c r="B64" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>143</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>148</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>149</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>152</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>155</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>157</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>